<commit_message>
Day 5 05042025 16h41 PM
</commit_message>
<xml_diff>
--- a/model_gemini.xlsx
+++ b/model_gemini.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\doft\dat\WebReactjs\converted_ai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7980823E-3589-4A51-9970-F1B5FFB58C47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0BAEE8-272A-47E4-990E-FC7CF525D386}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D9CA790-056C-4E5A-A5CA-DE3563CA9B83}"/>
+    <workbookView xWindow="10635" yWindow="45" windowWidth="10650" windowHeight="7875" xr2:uid="{6D9CA790-056C-4E5A-A5CA-DE3563CA9B83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Mô hình</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Gemini 2.0 Flash Experimental</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -192,15 +195,9 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -212,6 +209,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,178 +534,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB81650-0555-42E8-B5FE-2CF1AE6B4CAC}">
-  <dimension ref="B1:E12"/>
+  <dimension ref="C1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+    <row r="1" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="str">
+        <f>LOWER(D3)</f>
+        <v>gemini 2.0 flash-lite</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E3" s="1">
         <v>30</v>
       </c>
-      <c r="D3" s="2">
+      <c r="F3" s="2">
         <v>1000000</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="10" t="str">
+        <f t="shared" ref="C4:C12" si="0">LOWER(D4)</f>
+        <v>gemma 3</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E4" s="1">
         <v>30</v>
       </c>
-      <c r="D4" s="2">
+      <c r="F4" s="2">
         <v>15000</v>
       </c>
-      <c r="E4" s="7">
+      <c r="G4" s="5">
         <v>14400</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini 2.0 flash</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E5" s="1">
         <v>15</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" s="2">
         <v>1000000</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini 1.5 flash</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1">
+      <c r="E6" s="1">
         <v>15</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F6" s="2">
         <v>1000000</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini 1.5 flash-8b</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
+      <c r="E7" s="1">
         <v>15</v>
       </c>
-      <c r="D7" s="2">
+      <c r="F7" s="2">
         <v>1000000</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini 2.0 flash experimental</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1">
+      <c r="E8" s="1">
         <v>10</v>
       </c>
-      <c r="D8" s="2">
+      <c r="F8" s="2">
         <v>1000000</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="G8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini 2.0 flash thinking experimental 01-21</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1">
+      <c r="E9" s="1">
         <v>10</v>
       </c>
-      <c r="D9" s="2">
+      <c r="F9" s="2">
         <v>4000000</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini 2.5 pro experimental</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="E10" s="1">
         <v>5</v>
       </c>
-      <c r="D10" s="2">
+      <c r="F10" s="2">
         <v>1000000</v>
       </c>
-      <c r="E10" s="6">
+      <c r="G10" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="3:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini embedding experimental 03-07</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1">
+      <c r="E11" s="1">
         <v>5</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="6">
+      <c r="G11" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>gemini 1.5 pro</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="1">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="F12" s="2">
         <v>32000</v>
       </c>
-      <c r="E12" s="6">
+      <c r="G12" s="4">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:E13">
-    <sortCondition descending="1" ref="C1:C13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:G13">
+    <sortCondition descending="1" ref="E1:E13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>